<commit_message>
Capitalisations of parent entities
</commit_message>
<xml_diff>
--- a/Population/BCIO_Population.xlsx
+++ b/Population/BCIO_Population.xlsx
@@ -851,7 +851,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Highest level of formal educational qualification achieved</t>
+          <t>highest level of formal educational qualification achieved</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Highest level of formal educational qualification achieved</t>
+          <t>highest level of formal educational qualification achieved</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Highest level of formal educational qualification achieved</t>
+          <t>highest level of formal educational qualification achieved</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Highest level of formal educational qualification achieved</t>
+          <t>highest level of formal educational qualification achieved</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Highest level of formal educational qualification achieved</t>
+          <t>highest level of formal educational qualification achieved</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Highest level of formal educational qualification achieved</t>
+          <t>highest level of formal educational qualification achieved</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Highest level of formal educational qualification achieved</t>
+          <t>highest level of formal educational qualification achieved</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Human population/ object aggregate</t>
+          <t>Human population</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>gender</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>gender</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr">
@@ -5717,7 +5717,7 @@
       </c>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>Member of a multi-person household</t>
+          <t>member of a multi-person household</t>
         </is>
       </c>
       <c r="D85" s="2" t="inlineStr">
@@ -6569,7 +6569,7 @@
       </c>
       <c r="C99" s="2" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>gender</t>
         </is>
       </c>
       <c r="D99" s="2" t="inlineStr">
@@ -8828,7 +8828,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tobacco-containing product user </t>
+          <t xml:space="preserve">tobacco-containing product user </t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -8856,7 +8856,11 @@
       <c r="V136" t="inlineStr"/>
       <c r="W136" t="inlineStr"/>
       <c r="X136" t="inlineStr"/>
-      <c r="Y136" t="inlineStr"/>
+      <c r="Y136" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
       <c r="Z136" t="inlineStr">
         <is>
           <t>External</t>

</xml_diff>